<commit_message>
latest excel sheet with Version and FA holi
</commit_message>
<xml_diff>
--- a/src/main/resources/Excelfiles/QA Enviornment.xlsx
+++ b/src/main/resources/Excelfiles/QA Enviornment.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Key</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Url</t>
-  </si>
-  <si>
-    <t>https://crewbidwebapp.firebaseapp.com/bidline</t>
   </si>
   <si>
     <t>https://crewbid-automation.firebaseapp.com/login</t>
@@ -1216,7 +1213,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1310,7 +1307,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>